<commit_message>
Gant task aangepast en chart aangemaakt
</commit_message>
<xml_diff>
--- a/Analyse/Gantt/Gantt Tasks.xlsx
+++ b/Analyse/Gantt/Gantt Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcsie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjarne\Desktop\DEP3\DataEngineeringP3\Analyse\Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4575C64F-F84F-48E8-83CF-4D75A1878CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8B4B1B-02CD-41E8-B6E2-FA6AA3D2C0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{5D368F5A-2A90-4EAF-90F3-752B18EA180C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D368F5A-2A90-4EAF-90F3-752B18EA180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Task</t>
   </si>
@@ -113,24 +113,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>Opzetten server met databank</t>
   </si>
   <si>
@@ -149,9 +131,6 @@
     <t>Webscraper, NBB en csv combineren in 1 script</t>
   </si>
   <si>
-    <t>D, E, F</t>
-  </si>
-  <si>
     <t>Script koppelen met databank (opslaan)</t>
   </si>
   <si>
@@ -171,6 +150,42 @@
   </si>
   <si>
     <t>Frontend Optimaliseren</t>
+  </si>
+  <si>
+    <t>Analyse UCD</t>
+  </si>
+  <si>
+    <t>Full-Text-Search gebruiken voor de score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webscraper Testen </t>
+  </si>
+  <si>
+    <t>NBB Scrapen Testen</t>
+  </si>
+  <si>
+    <t>Data Ophalen testen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t>Documentatie</t>
+  </si>
+  <si>
+    <t>E,G,I</t>
+  </si>
+  <si>
+    <t>J,K</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>M,P</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E, F, G, H, I, J, K, L, M, N, O, P ,Q, R,S</t>
   </si>
 </sst>
 </file>
@@ -245,7 +260,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -261,7 +276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,17 +572,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79902978-95C5-4A67-A7B2-9717B8F68890}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -578,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -589,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -600,24 +619,24 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -636,10 +655,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,13 +680,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,13 +694,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,10 +705,10 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -700,13 +719,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +733,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +747,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,87 +761,108 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>30</v>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>